<commit_message>
todo bien con las exportaciones
</commit_message>
<xml_diff>
--- a/src/assets/Usuarios de crownparadise.xlsx
+++ b/src/assets/Usuarios de crownparadise.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A0AF02-CF36-4C57-BCC9-EF634AE22BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C55AA0-20F6-4BC6-BE3F-474AC0B19EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1336,8 +1336,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>